<commit_message>
troubleshooting and development. Modified Conditions in metadata.xlsx, metadata.csv, and counts.csv Error with detecting batch effects. Not enough local memory.
</commit_message>
<xml_diff>
--- a/metadata.xlsx
+++ b/metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10917"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="V:\data\CyTOF Data\CpG-GpC Burn Mu Blood TL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnpulford/R/CpG_GpC_Batch_Correction/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BA2EC24-BFD8-4B84-A121-93D62022DC86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B729AF66-7061-884A-BD79-30A315148908}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="171">
   <si>
     <t>OmiqID</t>
   </si>
@@ -531,10 +531,13 @@
     <t>Burn</t>
   </si>
   <si>
-    <t>NA</t>
-  </si>
-  <si>
     <t>Natural Immune</t>
+  </si>
+  <si>
+    <t>Sham</t>
+  </si>
+  <si>
+    <t>Control</t>
   </si>
 </sst>
 </file>
@@ -854,17 +857,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="H77" sqref="H77"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="E80" sqref="E80"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="36.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -884,7 +887,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -904,7 +907,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -924,7 +927,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -944,7 +947,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -964,7 +967,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -984,7 +987,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -998,13 +1001,13 @@
         <v>165</v>
       </c>
       <c r="E7" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="F7">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -1018,13 +1021,13 @@
         <v>165</v>
       </c>
       <c r="E8" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="F8">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -1038,13 +1041,13 @@
         <v>165</v>
       </c>
       <c r="E9" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="F9">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -1058,13 +1061,13 @@
         <v>166</v>
       </c>
       <c r="E10" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F10">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -1078,13 +1081,13 @@
         <v>166</v>
       </c>
       <c r="E11" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F11">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -1092,7 +1095,7 @@
         <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D12" t="s">
         <v>165</v>
@@ -1104,7 +1107,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -1112,7 +1115,7 @@
         <v>25</v>
       </c>
       <c r="C13" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D13" t="s">
         <v>165</v>
@@ -1124,7 +1127,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -1132,7 +1135,7 @@
         <v>27</v>
       </c>
       <c r="C14" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D14" t="s">
         <v>166</v>
@@ -1144,7 +1147,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -1152,7 +1155,7 @@
         <v>29</v>
       </c>
       <c r="C15" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D15" t="s">
         <v>166</v>
@@ -1164,7 +1167,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -1172,7 +1175,7 @@
         <v>31</v>
       </c>
       <c r="C16" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D16" t="s">
         <v>166</v>
@@ -1184,7 +1187,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -1192,19 +1195,19 @@
         <v>33</v>
       </c>
       <c r="C17" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D17" t="s">
         <v>165</v>
       </c>
       <c r="E17" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="F17">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -1212,19 +1215,19 @@
         <v>35</v>
       </c>
       <c r="C18" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D18" t="s">
         <v>165</v>
       </c>
       <c r="E18" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="F18">
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -1232,19 +1235,19 @@
         <v>37</v>
       </c>
       <c r="C19" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D19" t="s">
         <v>165</v>
       </c>
       <c r="E19" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="F19">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -1252,19 +1255,19 @@
         <v>39</v>
       </c>
       <c r="C20" t="s">
+        <v>168</v>
+      </c>
+      <c r="D20" t="s">
+        <v>166</v>
+      </c>
+      <c r="E20" t="s">
         <v>169</v>
-      </c>
-      <c r="D20" t="s">
-        <v>166</v>
-      </c>
-      <c r="E20" t="s">
-        <v>168</v>
       </c>
       <c r="F20">
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>40</v>
       </c>
@@ -1272,19 +1275,19 @@
         <v>41</v>
       </c>
       <c r="C21" t="s">
+        <v>168</v>
+      </c>
+      <c r="D21" t="s">
+        <v>166</v>
+      </c>
+      <c r="E21" t="s">
         <v>169</v>
-      </c>
-      <c r="D21" t="s">
-        <v>166</v>
-      </c>
-      <c r="E21" t="s">
-        <v>168</v>
       </c>
       <c r="F21">
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>42</v>
       </c>
@@ -1304,7 +1307,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>44</v>
       </c>
@@ -1324,7 +1327,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>46</v>
       </c>
@@ -1344,7 +1347,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>48</v>
       </c>
@@ -1364,7 +1367,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>50</v>
       </c>
@@ -1384,7 +1387,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>52</v>
       </c>
@@ -1398,13 +1401,13 @@
         <v>165</v>
       </c>
       <c r="E27" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="F27">
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>54</v>
       </c>
@@ -1418,13 +1421,13 @@
         <v>165</v>
       </c>
       <c r="E28" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="F28">
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>56</v>
       </c>
@@ -1438,13 +1441,13 @@
         <v>166</v>
       </c>
       <c r="E29" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F29">
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>58</v>
       </c>
@@ -1458,13 +1461,13 @@
         <v>166</v>
       </c>
       <c r="E30" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F30">
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>60</v>
       </c>
@@ -1478,13 +1481,13 @@
         <v>166</v>
       </c>
       <c r="E31" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F31">
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>62</v>
       </c>
@@ -1492,7 +1495,7 @@
         <v>63</v>
       </c>
       <c r="C32" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D32" t="s">
         <v>165</v>
@@ -1504,7 +1507,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>64</v>
       </c>
@@ -1512,7 +1515,7 @@
         <v>65</v>
       </c>
       <c r="C33" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D33" t="s">
         <v>165</v>
@@ -1524,7 +1527,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>66</v>
       </c>
@@ -1532,7 +1535,7 @@
         <v>67</v>
       </c>
       <c r="C34" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D34" t="s">
         <v>165</v>
@@ -1544,7 +1547,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>68</v>
       </c>
@@ -1552,7 +1555,7 @@
         <v>69</v>
       </c>
       <c r="C35" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D35" t="s">
         <v>166</v>
@@ -1564,7 +1567,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>70</v>
       </c>
@@ -1572,7 +1575,7 @@
         <v>71</v>
       </c>
       <c r="C36" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D36" t="s">
         <v>166</v>
@@ -1584,7 +1587,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>72</v>
       </c>
@@ -1592,19 +1595,19 @@
         <v>73</v>
       </c>
       <c r="C37" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D37" t="s">
         <v>165</v>
       </c>
       <c r="E37" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="F37">
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>74</v>
       </c>
@@ -1612,19 +1615,19 @@
         <v>75</v>
       </c>
       <c r="C38" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D38" t="s">
         <v>165</v>
       </c>
       <c r="E38" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="F38">
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>76</v>
       </c>
@@ -1632,19 +1635,19 @@
         <v>77</v>
       </c>
       <c r="C39" t="s">
+        <v>168</v>
+      </c>
+      <c r="D39" t="s">
+        <v>166</v>
+      </c>
+      <c r="E39" t="s">
         <v>169</v>
-      </c>
-      <c r="D39" t="s">
-        <v>166</v>
-      </c>
-      <c r="E39" t="s">
-        <v>168</v>
       </c>
       <c r="F39">
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>78</v>
       </c>
@@ -1652,19 +1655,19 @@
         <v>79</v>
       </c>
       <c r="C40" t="s">
+        <v>168</v>
+      </c>
+      <c r="D40" t="s">
+        <v>166</v>
+      </c>
+      <c r="E40" t="s">
         <v>169</v>
-      </c>
-      <c r="D40" t="s">
-        <v>166</v>
-      </c>
-      <c r="E40" t="s">
-        <v>168</v>
       </c>
       <c r="F40">
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>80</v>
       </c>
@@ -1672,19 +1675,19 @@
         <v>81</v>
       </c>
       <c r="C41" t="s">
+        <v>168</v>
+      </c>
+      <c r="D41" t="s">
+        <v>166</v>
+      </c>
+      <c r="E41" t="s">
         <v>169</v>
-      </c>
-      <c r="D41" t="s">
-        <v>166</v>
-      </c>
-      <c r="E41" t="s">
-        <v>168</v>
       </c>
       <c r="F41">
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>82</v>
       </c>
@@ -1704,7 +1707,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>84</v>
       </c>
@@ -1724,7 +1727,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>86</v>
       </c>
@@ -1744,7 +1747,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>88</v>
       </c>
@@ -1764,7 +1767,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>90</v>
       </c>
@@ -1784,7 +1787,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>92</v>
       </c>
@@ -1804,7 +1807,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>94</v>
       </c>
@@ -1824,7 +1827,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>96</v>
       </c>
@@ -1844,7 +1847,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>98</v>
       </c>
@@ -1864,7 +1867,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>100</v>
       </c>
@@ -1884,7 +1887,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>102</v>
       </c>
@@ -1898,13 +1901,13 @@
         <v>165</v>
       </c>
       <c r="E52" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="F52">
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>104</v>
       </c>
@@ -1918,13 +1921,13 @@
         <v>165</v>
       </c>
       <c r="E53" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="F53">
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>106</v>
       </c>
@@ -1938,13 +1941,13 @@
         <v>165</v>
       </c>
       <c r="E54" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="F54">
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>108</v>
       </c>
@@ -1958,13 +1961,13 @@
         <v>165</v>
       </c>
       <c r="E55" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="F55">
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>110</v>
       </c>
@@ -1978,13 +1981,13 @@
         <v>165</v>
       </c>
       <c r="E56" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="F56">
         <v>3</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>112</v>
       </c>
@@ -1998,13 +2001,13 @@
         <v>166</v>
       </c>
       <c r="E57" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F57">
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>114</v>
       </c>
@@ -2018,13 +2021,13 @@
         <v>166</v>
       </c>
       <c r="E58" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F58">
         <v>3</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>116</v>
       </c>
@@ -2038,13 +2041,13 @@
         <v>166</v>
       </c>
       <c r="E59" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F59">
         <v>3</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>118</v>
       </c>
@@ -2058,13 +2061,13 @@
         <v>166</v>
       </c>
       <c r="E60" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F60">
         <v>3</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>120</v>
       </c>
@@ -2072,19 +2075,19 @@
         <v>121</v>
       </c>
       <c r="C61" t="s">
+        <v>168</v>
+      </c>
+      <c r="D61" t="s">
+        <v>166</v>
+      </c>
+      <c r="E61" t="s">
         <v>169</v>
-      </c>
-      <c r="D61" t="s">
-        <v>166</v>
-      </c>
-      <c r="E61" t="s">
-        <v>168</v>
       </c>
       <c r="F61">
         <v>3</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>122</v>
       </c>
@@ -2092,7 +2095,7 @@
         <v>123</v>
       </c>
       <c r="C62" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D62" t="s">
         <v>165</v>
@@ -2104,7 +2107,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>124</v>
       </c>
@@ -2112,7 +2115,7 @@
         <v>125</v>
       </c>
       <c r="C63" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D63" t="s">
         <v>165</v>
@@ -2124,7 +2127,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>126</v>
       </c>
@@ -2132,7 +2135,7 @@
         <v>127</v>
       </c>
       <c r="C64" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D64" t="s">
         <v>165</v>
@@ -2144,7 +2147,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>128</v>
       </c>
@@ -2152,7 +2155,7 @@
         <v>129</v>
       </c>
       <c r="C65" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D65" t="s">
         <v>165</v>
@@ -2164,7 +2167,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>130</v>
       </c>
@@ -2172,7 +2175,7 @@
         <v>131</v>
       </c>
       <c r="C66" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D66" t="s">
         <v>165</v>
@@ -2184,7 +2187,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>132</v>
       </c>
@@ -2192,7 +2195,7 @@
         <v>133</v>
       </c>
       <c r="C67" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D67" t="s">
         <v>166</v>
@@ -2204,7 +2207,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>134</v>
       </c>
@@ -2212,7 +2215,7 @@
         <v>135</v>
       </c>
       <c r="C68" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D68" t="s">
         <v>166</v>
@@ -2224,7 +2227,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>136</v>
       </c>
@@ -2232,7 +2235,7 @@
         <v>137</v>
       </c>
       <c r="C69" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D69" t="s">
         <v>166</v>
@@ -2244,7 +2247,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>138</v>
       </c>
@@ -2252,7 +2255,7 @@
         <v>139</v>
       </c>
       <c r="C70" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D70" t="s">
         <v>166</v>
@@ -2264,7 +2267,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>140</v>
       </c>
@@ -2272,7 +2275,7 @@
         <v>141</v>
       </c>
       <c r="C71" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D71" t="s">
         <v>166</v>
@@ -2284,7 +2287,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>142</v>
       </c>
@@ -2292,19 +2295,19 @@
         <v>143</v>
       </c>
       <c r="C72" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D72" t="s">
         <v>165</v>
       </c>
       <c r="E72" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="F72">
         <v>4</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>144</v>
       </c>
@@ -2312,19 +2315,19 @@
         <v>145</v>
       </c>
       <c r="C73" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D73" t="s">
         <v>165</v>
       </c>
       <c r="E73" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="F73">
         <v>4</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>146</v>
       </c>
@@ -2332,19 +2335,19 @@
         <v>147</v>
       </c>
       <c r="C74" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D74" t="s">
         <v>165</v>
       </c>
       <c r="E74" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="F74">
         <v>4</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>148</v>
       </c>
@@ -2352,19 +2355,19 @@
         <v>149</v>
       </c>
       <c r="C75" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D75" t="s">
         <v>165</v>
       </c>
       <c r="E75" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="F75">
         <v>4</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>150</v>
       </c>
@@ -2372,19 +2375,19 @@
         <v>151</v>
       </c>
       <c r="C76" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D76" t="s">
         <v>165</v>
       </c>
       <c r="E76" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="F76">
         <v>4</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>152</v>
       </c>
@@ -2392,19 +2395,19 @@
         <v>153</v>
       </c>
       <c r="C77" t="s">
+        <v>168</v>
+      </c>
+      <c r="D77" t="s">
+        <v>166</v>
+      </c>
+      <c r="E77" t="s">
         <v>169</v>
-      </c>
-      <c r="D77" t="s">
-        <v>166</v>
-      </c>
-      <c r="E77" t="s">
-        <v>168</v>
       </c>
       <c r="F77">
         <v>4</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>154</v>
       </c>
@@ -2412,19 +2415,19 @@
         <v>155</v>
       </c>
       <c r="C78" t="s">
+        <v>168</v>
+      </c>
+      <c r="D78" t="s">
+        <v>166</v>
+      </c>
+      <c r="E78" t="s">
         <v>169</v>
-      </c>
-      <c r="D78" t="s">
-        <v>166</v>
-      </c>
-      <c r="E78" t="s">
-        <v>168</v>
       </c>
       <c r="F78">
         <v>4</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>156</v>
       </c>
@@ -2432,19 +2435,19 @@
         <v>157</v>
       </c>
       <c r="C79" t="s">
+        <v>168</v>
+      </c>
+      <c r="D79" t="s">
+        <v>166</v>
+      </c>
+      <c r="E79" t="s">
         <v>169</v>
-      </c>
-      <c r="D79" t="s">
-        <v>166</v>
-      </c>
-      <c r="E79" t="s">
-        <v>168</v>
       </c>
       <c r="F79">
         <v>4</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>158</v>
       </c>
@@ -2452,13 +2455,13 @@
         <v>159</v>
       </c>
       <c r="C80" t="s">
+        <v>168</v>
+      </c>
+      <c r="D80" t="s">
+        <v>166</v>
+      </c>
+      <c r="E80" t="s">
         <v>169</v>
-      </c>
-      <c r="D80" t="s">
-        <v>166</v>
-      </c>
-      <c r="E80" t="s">
-        <v>168</v>
       </c>
       <c r="F80">
         <v>4</v>

</xml_diff>